<commit_message>
Started preprocess_SmartFall.py to get SmartFall dataset into the format that is compatible with the data we will get from the OSD watches.
</commit_message>
<xml_diff>
--- a/Datasets/Datasets.xlsx
+++ b/Datasets/Datasets.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Mauldin et al.</t>
   </si>
   <si>
-    <t xml:space="preserve">SmartFall – Android App</t>
+    <t xml:space="preserve">SmartFall – Android App – uses a relatively small RNN</t>
   </si>
   <si>
     <t xml:space="preserve">SmartFall – A Smartwatch based Fall Detection System using Deep Learning</t>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">Santos et al.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used a few different neural network configurations and proposes one that gives best performance.</t>
   </si>
   <si>
     <t xml:space="preserve">Accelerometer-Based Human Fall Detection Using Convolutional Neural Networks</t>
@@ -466,10 +469,10 @@
   </sheetPr>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -907,13 +910,15 @@
       <c r="D20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -928,17 +933,17 @@
         <v>2018</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>

</xml_diff>